<commit_message>
repeated semenar 6 tasks for myself
</commit_message>
<xml_diff>
--- a/seminars/sem6/ДЗ.xlsx
+++ b/seminars/sem6/ДЗ.xlsx
@@ -5,66 +5,70 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Legion\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Programming\excel_basics\seminars\sem6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADA45E31-D1E5-4D42-BA1B-852E1FEBF350}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65D3969B-AE0E-4E12-943D-A1EAAC9D110E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="3" xr2:uid="{99C698EB-E7D8-4048-97A8-59943F91D461}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{99C698EB-E7D8-4048-97A8-59943F91D461}"/>
   </bookViews>
   <sheets>
     <sheet name="ДЗ_1_1" sheetId="3" r:id="rId1"/>
     <sheet name="ДЗ_1_2" sheetId="4" r:id="rId2"/>
     <sheet name="Структура сценария ДЗ_1_2" sheetId="5" r:id="rId3"/>
-    <sheet name="ДЗ_2" sheetId="2" r:id="rId4"/>
-    <sheet name="Отчет о результатах 1" sheetId="6" r:id="rId5"/>
-    <sheet name="Отчет об устойчивости 1" sheetId="7" r:id="rId6"/>
-    <sheet name="Отчет о пределах 1" sheetId="8" r:id="rId7"/>
+    <sheet name="Отчет о результатах 2" sheetId="9" r:id="rId4"/>
+    <sheet name="Отчет об устойчивости 2" sheetId="10" r:id="rId5"/>
+    <sheet name="Отчет о пределах 2" sheetId="11" r:id="rId6"/>
+    <sheet name="ДЗ_2" sheetId="2" r:id="rId7"/>
+    <sheet name="Отчет о результатах 1" sheetId="6" r:id="rId8"/>
+    <sheet name="Отчет об устойчивости 1" sheetId="7" r:id="rId9"/>
+    <sheet name="Отчет о пределах 1" sheetId="8" r:id="rId10"/>
   </sheets>
   <definedNames>
-    <definedName name="solver_adj" localSheetId="3" hidden="1">ДЗ_2!$B$6,ДЗ_2!$C$6,ДЗ_2!$D$6</definedName>
-    <definedName name="solver_cvg" localSheetId="3" hidden="1">0.0001</definedName>
-    <definedName name="solver_drv" localSheetId="3" hidden="1">2</definedName>
-    <definedName name="solver_eng" localSheetId="3" hidden="1">2</definedName>
-    <definedName name="solver_est" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_itr" localSheetId="3" hidden="1">2147483647</definedName>
-    <definedName name="solver_lhs1" localSheetId="3" hidden="1">ДЗ_2!$E$9</definedName>
-    <definedName name="solver_lhs2" localSheetId="3" hidden="1">ДЗ_2!$E$10</definedName>
-    <definedName name="solver_lhs3" localSheetId="3" hidden="1">ДЗ_2!$E$10</definedName>
-    <definedName name="solver_lhs4" localSheetId="3" hidden="1">ДЗ_2!$E$10</definedName>
-    <definedName name="solver_lhs5" localSheetId="3" hidden="1">ДЗ_2!$E$10</definedName>
-    <definedName name="solver_mip" localSheetId="3" hidden="1">2147483647</definedName>
-    <definedName name="solver_mni" localSheetId="3" hidden="1">30</definedName>
-    <definedName name="solver_mrt" localSheetId="3" hidden="1">0.075</definedName>
-    <definedName name="solver_msl" localSheetId="3" hidden="1">2</definedName>
-    <definedName name="solver_neg" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_nod" localSheetId="3" hidden="1">2147483647</definedName>
-    <definedName name="solver_num" localSheetId="3" hidden="1">2</definedName>
-    <definedName name="solver_nwt" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="3" hidden="1">ДЗ_2!$B$8</definedName>
-    <definedName name="solver_pre" localSheetId="3" hidden="1">0.000001</definedName>
-    <definedName name="solver_rbv" localSheetId="3" hidden="1">2</definedName>
-    <definedName name="solver_rel1" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_rel2" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_rel3" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_rel4" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_rel5" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_rhs1" localSheetId="3" hidden="1">13000</definedName>
-    <definedName name="solver_rhs2" localSheetId="3" hidden="1">3000</definedName>
-    <definedName name="solver_rhs3" localSheetId="3" hidden="1">3000</definedName>
-    <definedName name="solver_rhs4" localSheetId="3" hidden="1">3000</definedName>
-    <definedName name="solver_rhs5" localSheetId="3" hidden="1">3000</definedName>
-    <definedName name="solver_rlx" localSheetId="3" hidden="1">2</definedName>
-    <definedName name="solver_rsd" localSheetId="3" hidden="1">0</definedName>
-    <definedName name="solver_scl" localSheetId="3" hidden="1">2</definedName>
-    <definedName name="solver_sho" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_adj" localSheetId="6" hidden="1">ДЗ_2!$B$6,ДЗ_2!$C$6,ДЗ_2!$D$6</definedName>
+    <definedName name="solver_cvg" localSheetId="6" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="6" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="6" hidden="1">2</definedName>
+    <definedName name="solver_est" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="6" hidden="1">2147483647</definedName>
+    <definedName name="solver_lhs1" localSheetId="6" hidden="1">ДЗ_2!$B$6:$D$6</definedName>
+    <definedName name="solver_lhs2" localSheetId="6" hidden="1">ДЗ_2!$E$9</definedName>
+    <definedName name="solver_lhs3" localSheetId="6" hidden="1">ДЗ_2!$E$10</definedName>
+    <definedName name="solver_lhs4" localSheetId="6" hidden="1">ДЗ_2!$E$10</definedName>
+    <definedName name="solver_lhs5" localSheetId="6" hidden="1">ДЗ_2!$E$10</definedName>
+    <definedName name="solver_mip" localSheetId="6" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="6" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="6" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="6" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="6" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="6" hidden="1">3</definedName>
+    <definedName name="solver_nwt" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_opt" localSheetId="6" hidden="1">ДЗ_2!$B$8</definedName>
+    <definedName name="solver_pre" localSheetId="6" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="6" hidden="1">2</definedName>
+    <definedName name="solver_rel1" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_rel2" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_rel3" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_rel4" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_rel5" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_rhs1" localSheetId="6" hidden="1">100%</definedName>
+    <definedName name="solver_rhs2" localSheetId="6" hidden="1">13000</definedName>
+    <definedName name="solver_rhs3" localSheetId="6" hidden="1">3000</definedName>
+    <definedName name="solver_rhs4" localSheetId="6" hidden="1">3000</definedName>
+    <definedName name="solver_rhs5" localSheetId="6" hidden="1">3000</definedName>
+    <definedName name="solver_rlx" localSheetId="6" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="6" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="6" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="6" hidden="1">2</definedName>
-    <definedName name="solver_ssz" localSheetId="3" hidden="1">100</definedName>
-    <definedName name="solver_tim" localSheetId="3" hidden="1">2147483647</definedName>
-    <definedName name="solver_tol" localSheetId="3" hidden="1">0.01</definedName>
-    <definedName name="solver_typ" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_val" localSheetId="3" hidden="1">0</definedName>
-    <definedName name="solver_ver" localSheetId="3" hidden="1">3</definedName>
+    <definedName name="solver_sho" localSheetId="9" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="5" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="6" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="6" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="6" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_val" localSheetId="6" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="6" hidden="1">3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -85,7 +89,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="101">
   <si>
     <t>Прибыль</t>
   </si>
@@ -361,13 +365,40 @@
   </si>
   <si>
     <t>Верхний</t>
+  </si>
+  <si>
+    <t>Лист: [ДЗ.xlsx]ДЗ_2</t>
+  </si>
+  <si>
+    <t>Отчет создан: 12/20/2023 5:59:05 PM</t>
+  </si>
+  <si>
+    <t>Время решения: 0.016 секунд.</t>
+  </si>
+  <si>
+    <t>Число итераций: 4 Число подзадач: 0</t>
+  </si>
+  <si>
+    <t>Максимальное время Без пределов,  Число итераций Без пределов, Precision 0.000001</t>
+  </si>
+  <si>
+    <t>$B$6&lt;=1</t>
+  </si>
+  <si>
+    <t>$C$6&lt;=1</t>
+  </si>
+  <si>
+    <t>$D$6&lt;=1</t>
+  </si>
+  <si>
+    <t>$B$6:$D$6 &lt;= 100%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -458,6 +489,23 @@
       <b/>
       <sz val="11"/>
       <color indexed="18"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="18"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -788,7 +836,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -860,9 +908,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -881,6 +926,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1009,7 +1069,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>58173</xdr:colOff>
+      <xdr:colOff>10548</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
@@ -1350,25 +1410,25 @@
       <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="25"/>
-    <col min="2" max="2" width="14.26953125" style="25" customWidth="1"/>
-    <col min="3" max="3" width="10.54296875" style="25" customWidth="1"/>
-    <col min="4" max="4" width="12.453125" style="25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.08984375" style="25" customWidth="1"/>
-    <col min="6" max="6" width="10.6328125" style="25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.7265625" style="25"/>
-    <col min="8" max="9" width="13.1796875" style="25" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.36328125" style="25" customWidth="1"/>
-    <col min="11" max="11" width="7.90625" style="25" customWidth="1"/>
-    <col min="12" max="12" width="10.1796875" style="25" customWidth="1"/>
-    <col min="13" max="13" width="9.36328125" style="25" customWidth="1"/>
-    <col min="14" max="14" width="10.453125" style="25" customWidth="1"/>
-    <col min="15" max="16384" width="8.7265625" style="25"/>
+    <col min="1" max="1" width="8.7109375" style="25"/>
+    <col min="2" max="2" width="14.28515625" style="25" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" style="25" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" style="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="25" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" style="25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" style="25"/>
+    <col min="8" max="9" width="13.140625" style="25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.42578125" style="25" customWidth="1"/>
+    <col min="11" max="11" width="7.85546875" style="25" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" style="25" customWidth="1"/>
+    <col min="13" max="13" width="9.42578125" style="25" customWidth="1"/>
+    <col min="14" max="14" width="10.42578125" style="25" customWidth="1"/>
+    <col min="15" max="16384" width="8.7109375" style="25"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" ht="41.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:14" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="31" t="s">
         <v>16</v>
       </c>
@@ -1388,7 +1448,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B3" s="27">
         <v>50000000</v>
       </c>
@@ -1409,17 +1469,17 @@
         <v>1866.25</v>
       </c>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="I4" s="49" t="s">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I4" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="J4" s="49"/>
-      <c r="K4" s="49"/>
-      <c r="L4" s="49"/>
-      <c r="M4" s="49"/>
-      <c r="N4" s="49"/>
-    </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="J4" s="63"/>
+      <c r="K4" s="63"/>
+      <c r="L4" s="63"/>
+      <c r="M4" s="63"/>
+      <c r="N4" s="63"/>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I5" s="32">
         <f>(E3*F3*D3*365*C3-B3)/1000000</f>
         <v>1866.25</v>
@@ -1440,7 +1500,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I6" s="33">
         <v>1</v>
       </c>
@@ -1461,7 +1521,7 @@
         <v>2249.5</v>
       </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I7" s="33">
         <v>2</v>
       </c>
@@ -1481,7 +1541,7 @@
         <v>4549</v>
       </c>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I8" s="33">
         <v>3</v>
       </c>
@@ -1501,7 +1561,7 @@
         <v>6848.5</v>
       </c>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I9" s="33">
         <v>4</v>
       </c>
@@ -1521,7 +1581,7 @@
         <v>9148</v>
       </c>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I10" s="33">
         <v>5</v>
       </c>
@@ -1586,6 +1646,190 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81CAE111-E6E7-49E5-B12F-53E0C66CCDC8}">
+  <dimension ref="A1:J15"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.140625" customWidth="1"/>
+    <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.140625" customWidth="1"/>
+    <col min="6" max="6" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.140625" customWidth="1"/>
+    <col min="9" max="9" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="52" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="52" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="52" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="61"/>
+      <c r="C6" s="61" t="s">
+        <v>77</v>
+      </c>
+      <c r="D6" s="61"/>
+    </row>
+    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="62" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="62" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="62" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="53" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" s="53" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="56">
+        <v>52000000.000000007</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="61"/>
+      <c r="C11" s="61" t="s">
+        <v>87</v>
+      </c>
+      <c r="D11" s="61"/>
+      <c r="F11" s="61" t="s">
+        <v>88</v>
+      </c>
+      <c r="G11" s="61" t="s">
+        <v>77</v>
+      </c>
+      <c r="I11" s="61" t="s">
+        <v>91</v>
+      </c>
+      <c r="J11" s="61" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="62" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="62" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="62" t="s">
+        <v>74</v>
+      </c>
+      <c r="F12" s="62" t="s">
+        <v>89</v>
+      </c>
+      <c r="G12" s="62" t="s">
+        <v>90</v>
+      </c>
+      <c r="I12" s="62" t="s">
+        <v>89</v>
+      </c>
+      <c r="J12" s="62" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="55" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" s="55" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="57">
+        <v>4.3333333333333339</v>
+      </c>
+      <c r="F13" s="57">
+        <v>0</v>
+      </c>
+      <c r="G13" s="57">
+        <v>0</v>
+      </c>
+      <c r="I13" s="57">
+        <v>4.333333333333333</v>
+      </c>
+      <c r="J13" s="57">
+        <v>51999999.999999993</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="55" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="55" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" s="57">
+        <v>0</v>
+      </c>
+      <c r="F14" s="57">
+        <v>0</v>
+      </c>
+      <c r="G14" s="57">
+        <v>52000000.000000007</v>
+      </c>
+      <c r="I14" s="57">
+        <v>-2.090792417868801E-16</v>
+      </c>
+      <c r="J14" s="57">
+        <v>52000000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="53" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="53" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" s="58">
+        <v>0</v>
+      </c>
+      <c r="F15" s="58">
+        <v>0</v>
+      </c>
+      <c r="G15" s="58">
+        <v>52000000.000000007</v>
+      </c>
+      <c r="I15" s="58">
+        <v>-6.8901113770676382E-16</v>
+      </c>
+      <c r="J15" s="58">
+        <v>52000000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{772A0530-C297-4F03-96F8-6AC12036B8F2}">
   <dimension ref="B2:N10"/>
@@ -1594,25 +1838,25 @@
       <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="25"/>
-    <col min="2" max="2" width="14.26953125" style="25" customWidth="1"/>
-    <col min="3" max="3" width="10.54296875" style="25" customWidth="1"/>
-    <col min="4" max="4" width="12.453125" style="25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.08984375" style="25" customWidth="1"/>
-    <col min="6" max="6" width="10.6328125" style="25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.7265625" style="25"/>
-    <col min="8" max="9" width="13.1796875" style="25" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.36328125" style="25" customWidth="1"/>
-    <col min="11" max="11" width="7.90625" style="25" customWidth="1"/>
-    <col min="12" max="12" width="10.1796875" style="25" customWidth="1"/>
-    <col min="13" max="13" width="9.36328125" style="25" customWidth="1"/>
-    <col min="14" max="14" width="10.453125" style="25" customWidth="1"/>
-    <col min="15" max="16384" width="8.7265625" style="25"/>
+    <col min="1" max="1" width="8.7109375" style="25"/>
+    <col min="2" max="2" width="14.28515625" style="25" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" style="25" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" style="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="25" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" style="25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" style="25"/>
+    <col min="8" max="9" width="13.140625" style="25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.42578125" style="25" customWidth="1"/>
+    <col min="11" max="11" width="7.85546875" style="25" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" style="25" customWidth="1"/>
+    <col min="13" max="13" width="9.42578125" style="25" customWidth="1"/>
+    <col min="14" max="14" width="10.42578125" style="25" customWidth="1"/>
+    <col min="15" max="16384" width="8.7109375" style="25"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" ht="41.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:14" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="31" t="s">
         <v>16</v>
       </c>
@@ -1632,7 +1876,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B3" s="27">
         <v>50000000</v>
       </c>
@@ -1653,17 +1897,17 @@
         <v>1866.25</v>
       </c>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="I4" s="49" t="s">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I4" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="J4" s="49"/>
-      <c r="K4" s="49"/>
-      <c r="L4" s="49"/>
-      <c r="M4" s="49"/>
-      <c r="N4" s="49"/>
-    </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="J4" s="63"/>
+      <c r="K4" s="63"/>
+      <c r="L4" s="63"/>
+      <c r="M4" s="63"/>
+      <c r="N4" s="63"/>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I5" s="32">
         <f>(E3*F3*D3*365*C3-B3)/1000000</f>
         <v>1866.25</v>
@@ -1684,7 +1928,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I6" s="33">
         <v>1</v>
       </c>
@@ -1705,7 +1949,7 @@
         <v>2249.5</v>
       </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I7" s="33">
         <v>2</v>
       </c>
@@ -1725,7 +1969,7 @@
         <v>4549</v>
       </c>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I8" s="33">
         <v>3</v>
       </c>
@@ -1745,7 +1989,7 @@
         <v>6848.5</v>
       </c>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I9" s="33">
         <v>4</v>
       </c>
@@ -1765,7 +2009,7 @@
         <v>9148</v>
       </c>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I10" s="33">
         <v>5</v>
       </c>
@@ -1852,14 +2096,14 @@
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="5.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="15.7265625" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="3" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="15.7109375" bestFit="1" customWidth="1" outlineLevel="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="39" t="s">
         <v>27</v>
       </c>
@@ -1869,7 +2113,7 @@
       <c r="F2" s="44"/>
       <c r="G2" s="44"/>
     </row>
-    <row r="3" spans="2:7" ht="15.5" collapsed="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:7" ht="15.75" collapsed="1" x14ac:dyDescent="0.25">
       <c r="B3" s="38"/>
       <c r="C3" s="38"/>
       <c r="D3" s="45" t="s">
@@ -1879,7 +2123,7 @@
       <c r="F3" s="45"/>
       <c r="G3" s="45"/>
     </row>
-    <row r="4" spans="2:7" ht="21" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:7" ht="22.5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B4" s="41"/>
       <c r="C4" s="41"/>
       <c r="D4" s="34"/>
@@ -1893,7 +2137,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="42" t="s">
         <v>28</v>
       </c>
@@ -1903,7 +2147,7 @@
       <c r="F5" s="40"/>
       <c r="G5" s="40"/>
     </row>
-    <row r="6" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B6" s="41"/>
       <c r="C6" s="41" t="s">
         <v>21</v>
@@ -1921,7 +2165,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="42" t="s">
         <v>30</v>
       </c>
@@ -1931,7 +2175,7 @@
       <c r="F7" s="40"/>
       <c r="G7" s="40"/>
     </row>
-    <row r="8" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B8" s="41"/>
       <c r="C8" s="41" t="s">
         <v>22</v>
@@ -1949,7 +2193,7 @@
         <v>1866.25</v>
       </c>
     </row>
-    <row r="9" spans="2:7" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="43"/>
       <c r="C9" s="43" t="s">
         <v>23</v>
@@ -1967,17 +2211,17 @@
         <v>1866.25</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>33</v>
       </c>
@@ -1988,23 +2232,783 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CD1324E-2841-4782-9044-1B46D02ED098}">
+  <dimension ref="A1:G34"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.28515625" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="52" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="52" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="52" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="52" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="52" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="52"/>
+      <c r="B6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="52"/>
+      <c r="B7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="52"/>
+      <c r="B8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="52" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" collapsed="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="64" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="64" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="64" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" s="64" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="53" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" s="53" t="s">
+        <v>58</v>
+      </c>
+      <c r="D16" s="56">
+        <v>52000000.000000007</v>
+      </c>
+      <c r="E16" s="56">
+        <v>48886666.666666672</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="64" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" s="64" t="s">
+        <v>48</v>
+      </c>
+      <c r="D20" s="64" t="s">
+        <v>49</v>
+      </c>
+      <c r="E20" s="64" t="s">
+        <v>50</v>
+      </c>
+      <c r="F20" s="64" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="55" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" s="55" t="s">
+        <v>60</v>
+      </c>
+      <c r="D21" s="57">
+        <v>4.3333333333333339</v>
+      </c>
+      <c r="E21" s="57">
+        <v>1</v>
+      </c>
+      <c r="F21" s="55" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="55" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" s="55" t="s">
+        <v>63</v>
+      </c>
+      <c r="D22" s="57">
+        <v>0</v>
+      </c>
+      <c r="E22" s="57">
+        <v>0.84597701149425297</v>
+      </c>
+      <c r="F22" s="55" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="53" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" s="53" t="s">
+        <v>65</v>
+      </c>
+      <c r="D23" s="58">
+        <v>0</v>
+      </c>
+      <c r="E23" s="58">
+        <v>1</v>
+      </c>
+      <c r="F23" s="53" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="64" t="s">
+        <v>47</v>
+      </c>
+      <c r="C27" s="64" t="s">
+        <v>48</v>
+      </c>
+      <c r="D27" s="64" t="s">
+        <v>53</v>
+      </c>
+      <c r="E27" s="64" t="s">
+        <v>54</v>
+      </c>
+      <c r="F27" s="64" t="s">
+        <v>55</v>
+      </c>
+      <c r="G27" s="64" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="55" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28" s="55" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" s="59">
+        <v>13000</v>
+      </c>
+      <c r="E28" s="55" t="s">
+        <v>67</v>
+      </c>
+      <c r="F28" s="55" t="s">
+        <v>68</v>
+      </c>
+      <c r="G28" s="55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="55" t="s">
+        <v>69</v>
+      </c>
+      <c r="C29" s="55" t="s">
+        <v>13</v>
+      </c>
+      <c r="D29" s="59">
+        <v>2389.3333333333335</v>
+      </c>
+      <c r="E29" s="55" t="s">
+        <v>70</v>
+      </c>
+      <c r="F29" s="55" t="s">
+        <v>71</v>
+      </c>
+      <c r="G29" s="55">
+        <v>610.66666666666652</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="65" t="s">
+        <v>100</v>
+      </c>
+      <c r="C30" s="55"/>
+      <c r="D30" s="59"/>
+      <c r="E30" s="55"/>
+      <c r="F30" s="55"/>
+      <c r="G30" s="55"/>
+    </row>
+    <row r="31" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="55" t="s">
+        <v>59</v>
+      </c>
+      <c r="C31" s="55" t="s">
+        <v>60</v>
+      </c>
+      <c r="D31" s="57">
+        <v>1</v>
+      </c>
+      <c r="E31" s="55" t="s">
+        <v>97</v>
+      </c>
+      <c r="F31" s="55" t="s">
+        <v>68</v>
+      </c>
+      <c r="G31" s="55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="55" t="s">
+        <v>62</v>
+      </c>
+      <c r="C32" s="55" t="s">
+        <v>63</v>
+      </c>
+      <c r="D32" s="57">
+        <v>0.84597701149425297</v>
+      </c>
+      <c r="E32" s="55" t="s">
+        <v>98</v>
+      </c>
+      <c r="F32" s="55" t="s">
+        <v>71</v>
+      </c>
+      <c r="G32" s="55">
+        <v>0.15402298850574703</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="53" t="s">
+        <v>64</v>
+      </c>
+      <c r="C33" s="53" t="s">
+        <v>65</v>
+      </c>
+      <c r="D33" s="58">
+        <v>1</v>
+      </c>
+      <c r="E33" s="53" t="s">
+        <v>99</v>
+      </c>
+      <c r="F33" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="G33" s="53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="34"/>
+      <c r="C34" s="34"/>
+      <c r="D34" s="35"/>
+      <c r="E34" s="34"/>
+      <c r="F34" s="34"/>
+      <c r="G34" s="34"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6F41476-35ED-44D3-9866-37284D145F2A}">
+  <dimension ref="A1:H17"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.28515625" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="52" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="52" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="52" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="66"/>
+      <c r="C7" s="66"/>
+      <c r="D7" s="66" t="s">
+        <v>73</v>
+      </c>
+      <c r="E7" s="66" t="s">
+        <v>75</v>
+      </c>
+      <c r="F7" s="66" t="s">
+        <v>77</v>
+      </c>
+      <c r="G7" s="66" t="s">
+        <v>79</v>
+      </c>
+      <c r="H7" s="66" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="67" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="67" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="67" t="s">
+        <v>74</v>
+      </c>
+      <c r="E8" s="67" t="s">
+        <v>76</v>
+      </c>
+      <c r="F8" s="67" t="s">
+        <v>78</v>
+      </c>
+      <c r="G8" s="67" t="s">
+        <v>80</v>
+      </c>
+      <c r="H8" s="67" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="55" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" s="55" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="55">
+        <v>1</v>
+      </c>
+      <c r="E9" s="55">
+        <v>999999.99999999814</v>
+      </c>
+      <c r="F9" s="55">
+        <v>12000000</v>
+      </c>
+      <c r="G9" s="55">
+        <v>1E+30</v>
+      </c>
+      <c r="H9" s="55">
+        <v>999999.99999999814</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="55" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="55" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" s="55">
+        <v>0.84597701149425297</v>
+      </c>
+      <c r="E10" s="55">
+        <v>0</v>
+      </c>
+      <c r="F10" s="55">
+        <v>31900000</v>
+      </c>
+      <c r="G10" s="55">
+        <v>725000</v>
+      </c>
+      <c r="H10" s="55">
+        <v>31900000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="53" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="53" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" s="53">
+        <v>1</v>
+      </c>
+      <c r="E11" s="53">
+        <v>220000</v>
+      </c>
+      <c r="F11" s="53">
+        <v>9900000</v>
+      </c>
+      <c r="G11" s="53">
+        <v>1E+30</v>
+      </c>
+      <c r="H11" s="53">
+        <v>220000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="66"/>
+      <c r="C14" s="66"/>
+      <c r="D14" s="66" t="s">
+        <v>73</v>
+      </c>
+      <c r="E14" s="66" t="s">
+        <v>82</v>
+      </c>
+      <c r="F14" s="66" t="s">
+        <v>84</v>
+      </c>
+      <c r="G14" s="66" t="s">
+        <v>79</v>
+      </c>
+      <c r="H14" s="66" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="67" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="67" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="67" t="s">
+        <v>74</v>
+      </c>
+      <c r="E15" s="67" t="s">
+        <v>83</v>
+      </c>
+      <c r="F15" s="67" t="s">
+        <v>85</v>
+      </c>
+      <c r="G15" s="67" t="s">
+        <v>80</v>
+      </c>
+      <c r="H15" s="67" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="55" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" s="55" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="55">
+        <v>13000</v>
+      </c>
+      <c r="E16" s="55">
+        <v>3666.6666666666665</v>
+      </c>
+      <c r="F16" s="55">
+        <v>13000</v>
+      </c>
+      <c r="G16" s="55">
+        <v>1339.9999999999991</v>
+      </c>
+      <c r="H16" s="55">
+        <v>7360.0000000000009</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" s="53" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="53">
+        <v>2389.3333333333335</v>
+      </c>
+      <c r="E17" s="53">
+        <v>0</v>
+      </c>
+      <c r="F17" s="53">
+        <v>3000</v>
+      </c>
+      <c r="G17" s="53">
+        <v>1E+30</v>
+      </c>
+      <c r="H17" s="53">
+        <v>610.66666666666674</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E740FCA-4C06-44A7-80C4-4E1230A787B8}">
+  <dimension ref="A1:J15"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection sqref="A1:A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.28515625" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.28515625" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.28515625" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="52" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="52" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="52" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="66"/>
+      <c r="C6" s="66" t="s">
+        <v>77</v>
+      </c>
+      <c r="D6" s="66"/>
+    </row>
+    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="67" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="67" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="67" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="53" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" s="53" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="56">
+        <v>48886666.666666672</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="66"/>
+      <c r="C11" s="66" t="s">
+        <v>87</v>
+      </c>
+      <c r="D11" s="66"/>
+      <c r="F11" s="66" t="s">
+        <v>88</v>
+      </c>
+      <c r="G11" s="66" t="s">
+        <v>77</v>
+      </c>
+      <c r="I11" s="66" t="s">
+        <v>91</v>
+      </c>
+      <c r="J11" s="66" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="67" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="67" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="67" t="s">
+        <v>74</v>
+      </c>
+      <c r="F12" s="67" t="s">
+        <v>89</v>
+      </c>
+      <c r="G12" s="67" t="s">
+        <v>90</v>
+      </c>
+      <c r="I12" s="67" t="s">
+        <v>89</v>
+      </c>
+      <c r="J12" s="67" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="55" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" s="55" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="57">
+        <v>1</v>
+      </c>
+      <c r="F13" s="57">
+        <v>0</v>
+      </c>
+      <c r="G13" s="57">
+        <v>36886666.666666672</v>
+      </c>
+      <c r="I13" s="57">
+        <v>1</v>
+      </c>
+      <c r="J13" s="57">
+        <v>48886666.666666672</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="55" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="55" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" s="57">
+        <v>0.84597701149425297</v>
+      </c>
+      <c r="F14" s="57">
+        <v>0</v>
+      </c>
+      <c r="G14" s="57">
+        <v>21900000</v>
+      </c>
+      <c r="I14" s="57">
+        <v>0.84597701149425286</v>
+      </c>
+      <c r="J14" s="57">
+        <v>48886666.666666664</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="53" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="53" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" s="58">
+        <v>1</v>
+      </c>
+      <c r="F15" s="58">
+        <v>0</v>
+      </c>
+      <c r="G15" s="58">
+        <v>38986666.666666672</v>
+      </c>
+      <c r="I15" s="58">
+        <v>1</v>
+      </c>
+      <c r="J15" s="58">
+        <v>48886666.666666672</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{195FCB7D-E739-43CB-B0F3-FC7DFBAC2375}">
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.90625" customWidth="1"/>
-    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="4" t="s">
         <v>1</v>
@@ -2019,7 +3023,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -2036,7 +3040,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -2053,7 +3057,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -2067,7 +3071,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -2081,86 +3085,86 @@
         <v>11000</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="50">
-        <v>4.3333333333333339</v>
-      </c>
-      <c r="C6" s="51">
-        <v>0</v>
-      </c>
-      <c r="D6" s="52">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B6" s="49">
+        <v>1</v>
+      </c>
+      <c r="C6" s="50">
+        <v>0.84597701149425297</v>
+      </c>
+      <c r="D6" s="51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="17">
         <f>B5*B6</f>
-        <v>65000.000000000007</v>
+        <v>15000</v>
       </c>
       <c r="C7" s="18">
         <f t="shared" ref="C7:D7" si="0">C5*C6</f>
-        <v>0</v>
+        <v>24533.333333333336</v>
       </c>
       <c r="D7" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>11000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="24" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="48">
         <f>SUMPRODUCT(B2:D2,B7:D7)</f>
-        <v>52000000.000000007</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+        <v>48886666.666666672</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="21">
         <f>B7*B3</f>
-        <v>13000.000000000002</v>
+        <v>3000</v>
       </c>
       <c r="C9" s="21">
-        <f t="shared" ref="C9:E9" si="1">C7*C3</f>
-        <v>0</v>
+        <f t="shared" ref="C9:D9" si="1">C7*C3</f>
+        <v>7360.0000000000009</v>
       </c>
       <c r="D9" s="21">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2640</v>
       </c>
       <c r="E9" s="22">
         <f>SUM(B9:D9)</f>
-        <v>13000.000000000002</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>13000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="23" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="18">
         <f>B7*B4</f>
-        <v>2600.0000000000005</v>
+        <v>600</v>
       </c>
       <c r="C10" s="18">
-        <f t="shared" ref="C10:E10" si="2">C7*C4</f>
-        <v>0</v>
+        <f t="shared" ref="C10:D10" si="2">C7*C4</f>
+        <v>1349.3333333333335</v>
       </c>
       <c r="D10" s="18">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>440</v>
       </c>
       <c r="E10" s="19">
         <f>SUM(B10:D10)</f>
-        <v>2600.0000000000005</v>
+        <v>2389.3333333333335</v>
       </c>
     </row>
   </sheetData>
@@ -2169,250 +3173,250 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0812560-BC49-42BB-BE95-03B196DA66B9}">
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" outlineLevelRow="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.1796875" customWidth="1"/>
-    <col min="2" max="2" width="7.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.140625" customWidth="1"/>
+    <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="53" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="52" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="53" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="52" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="53" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="52" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="53" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="52" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="53" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="52" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="53"/>
+    <row r="6" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="52"/>
       <c r="B6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="53"/>
+    <row r="7" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="52"/>
       <c r="B7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="53"/>
+    <row r="8" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="52"/>
       <c r="B8" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:5" collapsed="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="53" t="s">
+    <row r="9" spans="1:5" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="52" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:5" collapsed="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:5" collapsed="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="55" t="s">
+    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="54" t="s">
         <v>47</v>
       </c>
-      <c r="C15" s="55" t="s">
+      <c r="C15" s="54" t="s">
         <v>48</v>
       </c>
-      <c r="D15" s="55" t="s">
+      <c r="D15" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="E15" s="55" t="s">
+      <c r="E15" s="54" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="54" t="s">
+    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="53" t="s">
         <v>57</v>
       </c>
-      <c r="C16" s="54" t="s">
+      <c r="C16" s="53" t="s">
         <v>58</v>
       </c>
-      <c r="D16" s="57">
+      <c r="D16" s="56">
         <v>52000000.000000007</v>
       </c>
-      <c r="E16" s="57">
+      <c r="E16" s="56">
         <v>52000000.000000007</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B20" s="55" t="s">
+    <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="54" t="s">
         <v>47</v>
       </c>
-      <c r="C20" s="55" t="s">
+      <c r="C20" s="54" t="s">
         <v>48</v>
       </c>
-      <c r="D20" s="55" t="s">
+      <c r="D20" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="E20" s="55" t="s">
+      <c r="E20" s="54" t="s">
         <v>50</v>
       </c>
-      <c r="F20" s="55" t="s">
+      <c r="F20" s="54" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B21" s="56" t="s">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="55" t="s">
         <v>59</v>
       </c>
-      <c r="C21" s="56" t="s">
+      <c r="C21" s="55" t="s">
         <v>60</v>
       </c>
-      <c r="D21" s="58">
+      <c r="D21" s="57">
         <v>4.3333333333333339</v>
       </c>
-      <c r="E21" s="58">
+      <c r="E21" s="57">
         <v>4.3333333333333339</v>
       </c>
-      <c r="F21" s="56" t="s">
+      <c r="F21" s="55" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B22" s="56" t="s">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="55" t="s">
         <v>62</v>
       </c>
-      <c r="C22" s="56" t="s">
+      <c r="C22" s="55" t="s">
         <v>63</v>
       </c>
-      <c r="D22" s="58">
+      <c r="D22" s="57">
         <v>0</v>
       </c>
-      <c r="E22" s="58">
+      <c r="E22" s="57">
         <v>0</v>
       </c>
-      <c r="F22" s="56" t="s">
+      <c r="F22" s="55" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="54" t="s">
+    <row r="23" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="53" t="s">
         <v>64</v>
       </c>
-      <c r="C23" s="54" t="s">
+      <c r="C23" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D23" s="59">
+      <c r="D23" s="58">
         <v>0</v>
       </c>
-      <c r="E23" s="59">
+      <c r="E23" s="58">
         <v>0</v>
       </c>
-      <c r="F23" s="54" t="s">
+      <c r="F23" s="53" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B27" s="55" t="s">
+    <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="54" t="s">
         <v>47</v>
       </c>
-      <c r="C27" s="55" t="s">
+      <c r="C27" s="54" t="s">
         <v>48</v>
       </c>
-      <c r="D27" s="55" t="s">
+      <c r="D27" s="54" t="s">
         <v>53</v>
       </c>
-      <c r="E27" s="55" t="s">
+      <c r="E27" s="54" t="s">
         <v>54</v>
       </c>
-      <c r="F27" s="55" t="s">
+      <c r="F27" s="54" t="s">
         <v>55</v>
       </c>
-      <c r="G27" s="55" t="s">
+      <c r="G27" s="54" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B28" s="56" t="s">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="55" t="s">
         <v>66</v>
       </c>
-      <c r="C28" s="56" t="s">
+      <c r="C28" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="D28" s="60">
+      <c r="D28" s="59">
         <v>13000.000000000002</v>
       </c>
-      <c r="E28" s="56" t="s">
+      <c r="E28" s="55" t="s">
         <v>67</v>
       </c>
-      <c r="F28" s="56" t="s">
+      <c r="F28" s="55" t="s">
         <v>68</v>
       </c>
-      <c r="G28" s="56">
+      <c r="G28" s="55">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B29" s="54" t="s">
+    <row r="29" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="53" t="s">
         <v>69</v>
       </c>
-      <c r="C29" s="54" t="s">
+      <c r="C29" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="D29" s="61">
+      <c r="D29" s="60">
         <v>2600.0000000000005</v>
       </c>
-      <c r="E29" s="54" t="s">
+      <c r="E29" s="53" t="s">
         <v>70</v>
       </c>
-      <c r="F29" s="54" t="s">
+      <c r="F29" s="53" t="s">
         <v>71</v>
       </c>
-      <c r="G29" s="54">
+      <c r="G29" s="53">
         <v>399.99999999999955</v>
       </c>
     </row>
@@ -2421,428 +3425,246 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{249E4D33-349F-4C20-AF49-C2AC56EFA211}">
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.1796875" customWidth="1"/>
-    <col min="2" max="2" width="7.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.140625" customWidth="1"/>
+    <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="53" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="52" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="53" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="52" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="53" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="52" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B7" s="62"/>
-      <c r="C7" s="62"/>
-      <c r="D7" s="62" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="61"/>
+      <c r="C7" s="61"/>
+      <c r="D7" s="61" t="s">
         <v>73</v>
       </c>
-      <c r="E7" s="62" t="s">
+      <c r="E7" s="61" t="s">
         <v>75</v>
       </c>
-      <c r="F7" s="62" t="s">
+      <c r="F7" s="61" t="s">
         <v>77</v>
       </c>
-      <c r="G7" s="62" t="s">
+      <c r="G7" s="61" t="s">
         <v>79</v>
       </c>
-      <c r="H7" s="62" t="s">
+      <c r="H7" s="61" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="63" t="s">
+    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="62" t="s">
         <v>47</v>
       </c>
-      <c r="C8" s="63" t="s">
+      <c r="C8" s="62" t="s">
         <v>48</v>
       </c>
-      <c r="D8" s="63" t="s">
+      <c r="D8" s="62" t="s">
         <v>74</v>
       </c>
-      <c r="E8" s="63" t="s">
+      <c r="E8" s="62" t="s">
         <v>76</v>
       </c>
-      <c r="F8" s="63" t="s">
+      <c r="F8" s="62" t="s">
         <v>78</v>
       </c>
-      <c r="G8" s="63" t="s">
+      <c r="G8" s="62" t="s">
         <v>80</v>
       </c>
-      <c r="H8" s="63" t="s">
+      <c r="H8" s="62" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B9" s="56" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="55" t="s">
         <v>59</v>
       </c>
-      <c r="C9" s="56" t="s">
+      <c r="C9" s="55" t="s">
         <v>60</v>
       </c>
-      <c r="D9" s="56">
+      <c r="D9" s="55">
         <v>4.3333333333333339</v>
       </c>
-      <c r="E9" s="56">
+      <c r="E9" s="55">
         <v>0</v>
       </c>
-      <c r="F9" s="56">
+      <c r="F9" s="55">
         <v>12000000</v>
       </c>
-      <c r="G9" s="56">
+      <c r="G9" s="55">
         <v>1E+30</v>
       </c>
-      <c r="H9" s="56">
+      <c r="H9" s="55">
         <v>750000.00000000186</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B10" s="56" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="55" t="s">
         <v>62</v>
       </c>
-      <c r="C10" s="56" t="s">
+      <c r="C10" s="55" t="s">
         <v>63</v>
       </c>
-      <c r="D10" s="56">
+      <c r="D10" s="55">
         <v>0</v>
       </c>
-      <c r="E10" s="56">
+      <c r="E10" s="55">
         <v>-2900000.0000000056</v>
       </c>
-      <c r="F10" s="56">
+      <c r="F10" s="55">
         <v>31900000</v>
       </c>
-      <c r="G10" s="56">
+      <c r="G10" s="55">
         <v>2900000.0000000056</v>
       </c>
-      <c r="H10" s="56">
+      <c r="H10" s="55">
         <v>1E+30</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="54" t="s">
+    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="53" t="s">
         <v>64</v>
       </c>
-      <c r="C11" s="54" t="s">
+      <c r="C11" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D11" s="54">
+      <c r="D11" s="53">
         <v>0</v>
       </c>
-      <c r="E11" s="54">
+      <c r="E11" s="53">
         <v>-660000.00000000175</v>
       </c>
-      <c r="F11" s="54">
+      <c r="F11" s="53">
         <v>9900000</v>
       </c>
-      <c r="G11" s="54">
+      <c r="G11" s="53">
         <v>660000.00000000175</v>
       </c>
-      <c r="H11" s="54">
+      <c r="H11" s="53">
         <v>1E+30</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B14" s="62"/>
-      <c r="C14" s="62"/>
-      <c r="D14" s="62" t="s">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="61"/>
+      <c r="C14" s="61"/>
+      <c r="D14" s="61" t="s">
         <v>73</v>
       </c>
-      <c r="E14" s="62" t="s">
+      <c r="E14" s="61" t="s">
         <v>82</v>
       </c>
-      <c r="F14" s="62" t="s">
+      <c r="F14" s="61" t="s">
         <v>84</v>
       </c>
-      <c r="G14" s="62" t="s">
+      <c r="G14" s="61" t="s">
         <v>79</v>
       </c>
-      <c r="H14" s="62" t="s">
+      <c r="H14" s="61" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="63" t="s">
+    <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="62" t="s">
         <v>47</v>
       </c>
-      <c r="C15" s="63" t="s">
+      <c r="C15" s="62" t="s">
         <v>48</v>
       </c>
-      <c r="D15" s="63" t="s">
+      <c r="D15" s="62" t="s">
         <v>74</v>
       </c>
-      <c r="E15" s="63" t="s">
+      <c r="E15" s="62" t="s">
         <v>83</v>
       </c>
-      <c r="F15" s="63" t="s">
+      <c r="F15" s="62" t="s">
         <v>85</v>
       </c>
-      <c r="G15" s="63" t="s">
+      <c r="G15" s="62" t="s">
         <v>80</v>
       </c>
-      <c r="H15" s="63" t="s">
+      <c r="H15" s="62" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B16" s="56" t="s">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="55" t="s">
         <v>66</v>
       </c>
-      <c r="C16" s="56" t="s">
+      <c r="C16" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="56">
+      <c r="D16" s="55">
         <v>13000.000000000002</v>
       </c>
-      <c r="E16" s="56">
+      <c r="E16" s="55">
         <v>4000.0000000000005</v>
       </c>
-      <c r="F16" s="56">
+      <c r="F16" s="55">
         <v>13000</v>
       </c>
-      <c r="G16" s="56">
+      <c r="G16" s="55">
         <v>2000.0000000000016</v>
       </c>
-      <c r="H16" s="56">
+      <c r="H16" s="55">
         <v>13000</v>
       </c>
     </row>
-    <row r="17" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="54" t="s">
+    <row r="17" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="53" t="s">
         <v>69</v>
       </c>
-      <c r="C17" s="54" t="s">
+      <c r="C17" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="54">
+      <c r="D17" s="53">
         <v>2600.0000000000005</v>
       </c>
-      <c r="E17" s="54">
+      <c r="E17" s="53">
         <v>0</v>
       </c>
-      <c r="F17" s="54">
+      <c r="F17" s="53">
         <v>3000</v>
       </c>
-      <c r="G17" s="54">
+      <c r="G17" s="53">
         <v>1E+30</v>
       </c>
-      <c r="H17" s="54">
+      <c r="H17" s="53">
         <v>400.00000000000028</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81CAE111-E6E7-49E5-B12F-53E0C66CCDC8}">
-  <dimension ref="A1:J15"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="2.1796875" customWidth="1"/>
-    <col min="2" max="2" width="7.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="2.1796875" customWidth="1"/>
-    <col min="6" max="6" width="7.90625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="2.1796875" customWidth="1"/>
-    <col min="9" max="9" width="8.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.26953125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" s="53" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="53" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="53" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B6" s="62"/>
-      <c r="C6" s="62" t="s">
-        <v>77</v>
-      </c>
-      <c r="D6" s="62"/>
-    </row>
-    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="63" t="s">
-        <v>47</v>
-      </c>
-      <c r="C7" s="63" t="s">
-        <v>48</v>
-      </c>
-      <c r="D7" s="63" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="54" t="s">
-        <v>57</v>
-      </c>
-      <c r="C8" s="54" t="s">
-        <v>58</v>
-      </c>
-      <c r="D8" s="57">
-        <v>52000000.000000007</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B11" s="62"/>
-      <c r="C11" s="62" t="s">
-        <v>87</v>
-      </c>
-      <c r="D11" s="62"/>
-      <c r="F11" s="62" t="s">
-        <v>88</v>
-      </c>
-      <c r="G11" s="62" t="s">
-        <v>77</v>
-      </c>
-      <c r="I11" s="62" t="s">
-        <v>91</v>
-      </c>
-      <c r="J11" s="62" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="63" t="s">
-        <v>47</v>
-      </c>
-      <c r="C12" s="63" t="s">
-        <v>48</v>
-      </c>
-      <c r="D12" s="63" t="s">
-        <v>74</v>
-      </c>
-      <c r="F12" s="63" t="s">
-        <v>89</v>
-      </c>
-      <c r="G12" s="63" t="s">
-        <v>90</v>
-      </c>
-      <c r="I12" s="63" t="s">
-        <v>89</v>
-      </c>
-      <c r="J12" s="63" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B13" s="56" t="s">
-        <v>59</v>
-      </c>
-      <c r="C13" s="56" t="s">
-        <v>60</v>
-      </c>
-      <c r="D13" s="58">
-        <v>4.3333333333333339</v>
-      </c>
-      <c r="F13" s="58">
-        <v>0</v>
-      </c>
-      <c r="G13" s="58">
-        <v>0</v>
-      </c>
-      <c r="I13" s="58">
-        <v>4.333333333333333</v>
-      </c>
-      <c r="J13" s="58">
-        <v>51999999.999999993</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B14" s="56" t="s">
-        <v>62</v>
-      </c>
-      <c r="C14" s="56" t="s">
-        <v>63</v>
-      </c>
-      <c r="D14" s="58">
-        <v>0</v>
-      </c>
-      <c r="F14" s="58">
-        <v>0</v>
-      </c>
-      <c r="G14" s="58">
-        <v>52000000.000000007</v>
-      </c>
-      <c r="I14" s="58">
-        <v>-2.090792417868801E-16</v>
-      </c>
-      <c r="J14" s="58">
-        <v>52000000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="54" t="s">
-        <v>64</v>
-      </c>
-      <c r="C15" s="54" t="s">
-        <v>65</v>
-      </c>
-      <c r="D15" s="59">
-        <v>0</v>
-      </c>
-      <c r="F15" s="59">
-        <v>0</v>
-      </c>
-      <c r="G15" s="59">
-        <v>52000000.000000007</v>
-      </c>
-      <c r="I15" s="59">
-        <v>-6.8901113770676382E-16</v>
-      </c>
-      <c r="J15" s="59">
-        <v>52000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>